<commit_message>
Actualizadas las tablas que faltan, falta actualizar la documentacion
</commit_message>
<xml_diff>
--- a/Taller3_12_re.gonzalez10_ja.troconis10/docs/tablas.xlsx
+++ b/Taller3_12_re.gonzalez10_ja.troconis10/docs/tablas.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ricardo\Documents\SisTrans_VuelAndes_C12\Taller3_12_re.gonzalez10_ja.troconis10\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JavierAntonio\git\SisTrans_VuelAndes_C12\Taller3_12_re.gonzalez10_ja.troconis10\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384"/>
+    <workbookView xWindow="930" yWindow="0" windowWidth="23040" windowHeight="9390"/>
   </bookViews>
   <sheets>
     <sheet name="Esquema de Relación" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="171">
   <si>
     <t>PK</t>
   </si>
@@ -413,12 +413,132 @@
   </si>
   <si>
     <t>FK(tiposviaje.id_tipo)</t>
+  </si>
+  <si>
+    <t>tipoId</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>PK2,ND</t>
+  </si>
+  <si>
+    <t>rol</t>
+  </si>
+  <si>
+    <t>FK(roles.id)</t>
+  </si>
+  <si>
+    <t>Roles</t>
+  </si>
+  <si>
+    <t>id_rol</t>
+  </si>
+  <si>
+    <t>Pasajeros</t>
+  </si>
+  <si>
+    <t>id_usuario</t>
+  </si>
+  <si>
+    <t>Usuarios</t>
+  </si>
+  <si>
+    <t>PK2,FK(Usuarios.id)</t>
+  </si>
+  <si>
+    <t>PK1,FK(Usuarios.tipoid)</t>
+  </si>
+  <si>
+    <t>PK1,FK(TiposId.tipoId)</t>
+  </si>
+  <si>
+    <t>TiposId</t>
+  </si>
+  <si>
+    <t>descripcion</t>
+  </si>
+  <si>
+    <t>frecuente</t>
+  </si>
+  <si>
+    <t>Remitentes</t>
+  </si>
+  <si>
+    <t>Cargas</t>
+  </si>
+  <si>
+    <t>contenido</t>
+  </si>
+  <si>
+    <t>peso</t>
+  </si>
+  <si>
+    <t>NN,CK(&gt;0)</t>
+  </si>
+  <si>
+    <t>volumen</t>
+  </si>
+  <si>
+    <t>ReservasCargas</t>
+  </si>
+  <si>
+    <t>carga</t>
+  </si>
+  <si>
+    <t>FK(Usuarios.tipoid)</t>
+  </si>
+  <si>
+    <t>FK(Usuarios.id)</t>
+  </si>
+  <si>
+    <t>vuelo</t>
+  </si>
+  <si>
+    <t>FK(Cargas.id)</t>
+  </si>
+  <si>
+    <t>FK(Vuelos.id_vuelo)</t>
+  </si>
+  <si>
+    <t>FK(Remitentes.tipoid)</t>
+  </si>
+  <si>
+    <t>FK(Remitentes.id)</t>
+  </si>
+  <si>
+    <t>ReservasPsajeros</t>
+  </si>
+  <si>
+    <t>FK(Pasajeros.tipoid)</t>
+  </si>
+  <si>
+    <t>FK(Pasajeros.id)</t>
+  </si>
+  <si>
+    <t>ViajerosFrecuentes</t>
+  </si>
+  <si>
+    <t>aerolinea</t>
+  </si>
+  <si>
+    <t>PK1,FK(Aerolinea.codIATA)</t>
+  </si>
+  <si>
+    <t>Nacionalidades</t>
+  </si>
+  <si>
+    <t>pais</t>
+  </si>
+  <si>
+    <t>FK(Paises.cod_pais)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -678,7 +798,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -708,6 +828,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -726,11 +847,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -746,7 +867,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -821,6 +942,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -856,6 +994,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1032,30 +1187,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L31"/>
+  <dimension ref="A1:L63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.33203125" customWidth="1"/>
+    <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" customWidth="1"/>
     <col min="4" max="4" width="25" customWidth="1"/>
-    <col min="5" max="5" width="26.109375" customWidth="1"/>
-    <col min="6" max="6" width="29.44140625" customWidth="1"/>
-    <col min="7" max="7" width="27.21875" customWidth="1"/>
+    <col min="5" max="5" width="26.140625" customWidth="1"/>
+    <col min="6" max="6" width="29.42578125" customWidth="1"/>
+    <col min="7" max="7" width="27.28515625" customWidth="1"/>
     <col min="8" max="8" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>25</v>
       </c>
@@ -1072,7 +1227,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>47</v>
       </c>
@@ -1089,12 +1244,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>23</v>
       </c>
@@ -1132,7 +1287,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
@@ -1170,12 +1325,12 @@
         <v>113</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="18" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>10</v>
       </c>
@@ -1189,7 +1344,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>21</v>
       </c>
@@ -1203,12 +1358,12 @@
         <v>115</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="18" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>10</v>
       </c>
@@ -1216,7 +1371,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>21</v>
       </c>
@@ -1224,20 +1379,20 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A17" s="11" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="25" t="s">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="B18" s="25" t="s">
+      <c r="B18" s="19" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>125</v>
       </c>
@@ -1245,23 +1400,23 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A21" s="11" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="25" t="s">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="19" t="s">
         <v>122</v>
       </c>
-      <c r="B22" s="25" t="s">
+      <c r="B22" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="25" t="s">
+      <c r="C22" s="19" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>125</v>
       </c>
@@ -1272,10 +1427,10 @@
         <v>124</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A24" s="11"/>
     </row>
-    <row r="25" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A25" s="11" t="s">
         <v>117</v>
       </c>
@@ -1283,7 +1438,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
         <v>121</v>
       </c>
@@ -1297,7 +1452,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>21</v>
       </c>
@@ -1311,12 +1466,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A29" s="11" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
         <v>121</v>
       </c>
@@ -1324,12 +1479,282 @@
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A33" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="F33" s="11" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="C34" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="D34" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="F34" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="G34" s="10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A37" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="F37" s="11" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="C38" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="F38" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="G38" s="10" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A41" s="11" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="B42" s="10" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A45" s="11" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="B46" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="C46" s="19" t="s">
+        <v>150</v>
+      </c>
+      <c r="D46" s="19" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A49" s="11" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="B50" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="C50" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="D50" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="E50" s="19" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E51" s="26" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A53" s="11" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="B54" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="C54" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="D54" s="19" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="D55" s="26" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A57" s="11" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="B58" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="C58" s="10" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A61" s="11" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="B62" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="C62" s="19" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -1343,46 +1768,46 @@
   <dimension ref="A1:H39"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:D39"/>
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="20"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C1" s="20"/>
+      <c r="D1" s="21"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="21"/>
-      <c r="D2" s="22"/>
-    </row>
-    <row r="3" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C2" s="22"/>
+      <c r="D2" s="23"/>
+    </row>
+    <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="23"/>
-      <c r="D3" s="24"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C3" s="24"/>
+      <c r="D3" s="25"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>5</v>
       </c>
@@ -1396,7 +1821,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>10</v>
       </c>
@@ -1410,7 +1835,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>20</v>
       </c>
@@ -1424,7 +1849,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>12</v>
       </c>
@@ -1438,7 +1863,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>13</v>
       </c>
@@ -1455,7 +1880,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G9" s="18" t="s">
         <v>0</v>
       </c>
@@ -1463,15 +1888,15 @@
         <v>72</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="19"/>
-      <c r="D10" s="20"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="21"/>
       <c r="G10" s="1" t="s">
         <v>71</v>
       </c>
@@ -1479,15 +1904,15 @@
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="21" t="s">
+      <c r="B11" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="21"/>
-      <c r="D11" s="22"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="23"/>
       <c r="G11" s="1" t="s">
         <v>1</v>
       </c>
@@ -1495,15 +1920,15 @@
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="23" t="s">
+      <c r="B12" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="C12" s="23"/>
-      <c r="D12" s="24"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="25"/>
       <c r="G12" s="1" t="s">
         <v>66</v>
       </c>
@@ -1511,7 +1936,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>5</v>
       </c>
@@ -1531,7 +1956,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>10</v>
       </c>
@@ -1551,7 +1976,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>20</v>
       </c>
@@ -1571,7 +1996,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G16" s="1" t="s">
         <v>70</v>
       </c>
@@ -1579,37 +2004,37 @@
         <v>79</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B17" s="19" t="s">
+      <c r="B17" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="C17" s="19"/>
-      <c r="D17" s="20"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C17" s="20"/>
+      <c r="D17" s="21"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B18" s="21" t="s">
+      <c r="B18" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="C18" s="21"/>
-      <c r="D18" s="22"/>
-    </row>
-    <row r="19" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C18" s="22"/>
+      <c r="D18" s="23"/>
+    </row>
+    <row r="19" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B19" s="23" t="s">
+      <c r="B19" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="C19" s="23"/>
-      <c r="D19" s="24"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C19" s="24"/>
+      <c r="D19" s="25"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>5</v>
       </c>
@@ -1623,7 +2048,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>32</v>
       </c>
@@ -1637,7 +2062,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>25</v>
       </c>
@@ -1651,7 +2076,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>26</v>
       </c>
@@ -1665,7 +2090,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
         <v>27</v>
       </c>
@@ -1685,7 +2110,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
         <v>28</v>
       </c>
@@ -1705,7 +2130,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
         <v>35</v>
       </c>
@@ -1719,38 +2144,38 @@
         <v>94</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B28" s="19" t="s">
+      <c r="B28" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="C28" s="19"/>
-      <c r="D28" s="20"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C28" s="20"/>
+      <c r="D28" s="21"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B29" s="21" t="s">
+      <c r="B29" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="C29" s="21"/>
-      <c r="D29" s="22"/>
-    </row>
-    <row r="30" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C29" s="22"/>
+      <c r="D29" s="23"/>
+    </row>
+    <row r="30" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B30" s="23" t="s">
+      <c r="B30" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="C30" s="23"/>
-      <c r="D30" s="24"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C30" s="24"/>
+      <c r="D30" s="25"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
         <v>5</v>
       </c>
@@ -1764,7 +2189,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="15" t="s">
         <v>23</v>
       </c>
@@ -1778,7 +2203,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>30</v>
       </c>
@@ -1792,7 +2217,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>31</v>
       </c>
@@ -1806,7 +2231,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>33</v>
       </c>
@@ -1820,7 +2245,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="16" t="s">
         <v>35</v>
       </c>
@@ -1834,7 +2259,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>38</v>
       </c>
@@ -1848,7 +2273,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
         <v>39</v>
       </c>
@@ -1862,7 +2287,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
         <v>80</v>
       </c>

</xml_diff>

<commit_message>
Se actualizaron unos pequeños detalles en las tablas, aun falta la documentacion
</commit_message>
<xml_diff>
--- a/Taller3_12_re.gonzalez10_ja.troconis10/docs/tablas.xlsx
+++ b/Taller3_12_re.gonzalez10_ja.troconis10/docs/tablas.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JavierAntonio\git\SisTrans_VuelAndes_C12\Taller3_12_re.gonzalez10_ja.troconis10\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ricardo\Documents\SisTrans_VuelAndes_C12\Taller3_12_re.gonzalez10_ja.troconis10\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="23040" windowHeight="9390"/>
+    <workbookView xWindow="936" yWindow="0" windowWidth="23040" windowHeight="9396"/>
   </bookViews>
   <sheets>
     <sheet name="Esquema de Relación" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="181">
   <si>
     <t>PK</t>
   </si>
@@ -286,9 +286,6 @@
     <t>FK(aerolineas.codIATA),UA,NN</t>
   </si>
   <si>
-    <t>FK(aeropuertos.codIATA),UA,NN</t>
-  </si>
-  <si>
     <t>FK(aerolineas.codIATA),UA</t>
   </si>
   <si>
@@ -334,12 +331,6 @@
     <t>NULLABEL</t>
   </si>
   <si>
-    <t>avion_asig</t>
-  </si>
-  <si>
-    <t>hacer FK</t>
-  </si>
-  <si>
     <t>hora_Salida</t>
   </si>
   <si>
@@ -364,21 +355,12 @@
     <t>NN, CK(1&gt;=frecuencia&lt;=7)</t>
   </si>
   <si>
-    <t>FK(ciudades.id)</t>
-  </si>
-  <si>
-    <t>FK(tiposaeropuertos.id)</t>
-  </si>
-  <si>
     <t>ciudad</t>
   </si>
   <si>
     <t>tiposAeropuertos</t>
   </si>
   <si>
-    <t>tiposVuelo</t>
-  </si>
-  <si>
     <t>Paises</t>
   </si>
   <si>
@@ -400,21 +382,12 @@
     <t>PK,UA</t>
   </si>
   <si>
-    <t>tiposViaje</t>
-  </si>
-  <si>
     <t>tipo_vuelo</t>
   </si>
   <si>
-    <t>FK(tiposvuelo.id_tipo)</t>
-  </si>
-  <si>
     <t>tipo_viaje</t>
   </si>
   <si>
-    <t>FK(tiposviaje.id_tipo)</t>
-  </si>
-  <si>
     <t>tipoId</t>
   </si>
   <si>
@@ -508,9 +481,6 @@
     <t>FK(Remitentes.id)</t>
   </si>
   <si>
-    <t>ReservasPsajeros</t>
-  </si>
-  <si>
     <t>FK(Pasajeros.tipoid)</t>
   </si>
   <si>
@@ -533,12 +503,72 @@
   </si>
   <si>
     <t>FK(Paises.cod_pais)</t>
+  </si>
+  <si>
+    <t>numero_de_serie</t>
+  </si>
+  <si>
+    <t>avion_asignado</t>
+  </si>
+  <si>
+    <t>codIATA_aeropuertoPartida</t>
+  </si>
+  <si>
+    <t>codIATA_aeropuertoLLegada</t>
+  </si>
+  <si>
+    <t>FK(aviones.numero_de_serie)</t>
+  </si>
+  <si>
+    <t>FK(aeropuertos.codIATA),UA,NN,CK(codIATA_aeropuertoPartida!=codIATA_aeropuertoLLegada)</t>
+  </si>
+  <si>
+    <t>FK(tiposvuelos.id_tipo)</t>
+  </si>
+  <si>
+    <t>FK(tiposviajes.id_tipo)</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>clasificacion</t>
+  </si>
+  <si>
+    <t>FK(ciudades.codigo_ciudad)</t>
+  </si>
+  <si>
+    <t>FK(tiposaeropuertos.id_tipo)</t>
+  </si>
+  <si>
+    <t>tiposVuelos</t>
+  </si>
+  <si>
+    <t>tiposViajes</t>
+  </si>
+  <si>
+    <t>tiposAviones</t>
+  </si>
+  <si>
+    <t>FK(tiposaviones.id_tipo)</t>
+  </si>
+  <si>
+    <t>tipo_avion</t>
+  </si>
+  <si>
+    <t>PK,UA(viene con el avion)</t>
+  </si>
+  <si>
+    <t>clave</t>
+  </si>
+  <si>
+    <t>ReservasPasajeros</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -829,6 +859,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -847,11 +878,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
+    <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -867,7 +897,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -942,23 +972,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -994,23 +1007,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1189,45 +1185,54 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="C63" sqref="C63"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.28515625" customWidth="1"/>
+    <col min="1" max="1" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.33203125" customWidth="1"/>
     <col min="4" max="4" width="25" customWidth="1"/>
-    <col min="5" max="5" width="26.140625" customWidth="1"/>
-    <col min="6" max="6" width="29.42578125" customWidth="1"/>
-    <col min="7" max="7" width="27.28515625" customWidth="1"/>
+    <col min="5" max="5" width="26.109375" customWidth="1"/>
+    <col min="6" max="6" width="29.44140625" customWidth="1"/>
+    <col min="7" max="7" width="27.33203125" customWidth="1"/>
     <col min="8" max="8" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>25</v>
       </c>
       <c r="B2" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="C2" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="D2" s="10" t="s">
         <v>100</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>101</v>
       </c>
       <c r="E2" s="10" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F2" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>47</v>
       </c>
@@ -1235,59 +1240,68 @@
         <v>47</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>103</v>
-      </c>
       <c r="E3" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+        <v>88</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="18" x14ac:dyDescent="0.35">
       <c r="A5" s="11" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>23</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>104</v>
+        <v>162</v>
       </c>
       <c r="E6" s="10" t="s">
         <v>35</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>38</v>
+        <v>163</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>39</v>
+        <v>164</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="I6" s="10" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="J6" s="10" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="K6" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="L6" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="L6" s="10" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
@@ -1298,39 +1312,42 @@
         <v>36</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>105</v>
+        <v>165</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>87</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>88</v>
+        <v>166</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>88</v>
+        <v>166</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>130</v>
+        <v>167</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>128</v>
+        <v>168</v>
       </c>
       <c r="J7" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="L7" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="K7" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:12" ht="18" x14ac:dyDescent="0.35">
       <c r="A9" s="11" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
         <v>10</v>
       </c>
@@ -1338,13 +1355,13 @@
         <v>20</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>21</v>
       </c>
@@ -1352,107 +1369,128 @@
         <v>22</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>114</v>
+        <v>171</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="18" x14ac:dyDescent="0.35">
       <c r="A13" s="11" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
         <v>10</v>
       </c>
       <c r="B14" s="10" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C14" s="19" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C15" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A17" s="11" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+      <c r="B17" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="19" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="B18" s="19" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A21" s="11" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+      <c r="B21" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="19" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="B22" s="19" t="s">
         <v>20</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A24" s="11"/>
     </row>
-    <row r="25" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A25" s="11" t="s">
-        <v>117</v>
+        <v>112</v>
+      </c>
+      <c r="B25" t="s">
+        <v>169</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+        <v>173</v>
+      </c>
+      <c r="E25" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="10" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="B26" s="10" t="s">
         <v>20</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="E26" s="10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>21</v>
       </c>
@@ -1466,158 +1504,200 @@
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A29" s="11" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+        <v>174</v>
+      </c>
+      <c r="B29" t="s">
+        <v>169</v>
+      </c>
+      <c r="D29" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="E29" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="10" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="B30" s="10" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D30" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="E30" s="10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D31" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A33" s="11" t="s">
-        <v>140</v>
-      </c>
-      <c r="F33" s="11" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="10" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="C34" s="19" t="s">
         <v>20</v>
       </c>
       <c r="D34" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="E34" s="19" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="F34" s="10" t="s">
-        <v>137</v>
-      </c>
-      <c r="G34" s="10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
-        <v>143</v>
-      </c>
       <c r="B35" s="1" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G35" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+        <v>126</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A37" s="11" t="s">
-        <v>138</v>
-      </c>
-      <c r="F37" s="11" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+      <c r="B37" t="s">
+        <v>169</v>
+      </c>
+      <c r="E37" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="F37" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="19" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="C38" s="10" t="s">
-        <v>146</v>
+        <v>137</v>
+      </c>
+      <c r="E38" s="10" t="s">
+        <v>128</v>
       </c>
       <c r="F38" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="G38" s="10" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="E39" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="F39" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="A41" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="B41" t="s">
+        <v>169</v>
+      </c>
+      <c r="E41" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="F41" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="B42" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="E42" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="F42" s="10" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="E43" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G39" s="1" t="s">
+      <c r="F43" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A41" s="11" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="19" t="s">
-        <v>131</v>
-      </c>
-      <c r="B42" s="10" t="s">
+    <row r="45" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="A45" s="11" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="B43" s="1" t="s">
+      <c r="B45" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="B46" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="C46" s="19" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A45" s="11" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="B46" s="10" t="s">
-        <v>149</v>
-      </c>
-      <c r="C46" s="19" t="s">
-        <v>150</v>
-      </c>
       <c r="D46" s="19" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>0</v>
       </c>
@@ -1625,136 +1705,148 @@
         <v>1</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A49" s="11" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+      <c r="B49" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="19" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="B50" s="19" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="C50" s="10" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="D50" s="10" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="E50" s="19" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="E51" s="26" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+        <v>149</v>
+      </c>
+      <c r="E51" s="20" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A53" s="11" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+      <c r="B53" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="19" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="B54" s="19" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="C54" s="10" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="D54" s="19" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="D55" s="26" t="s">
+        <v>154</v>
+      </c>
+      <c r="D55" s="20" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="A57" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="B57" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A58" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="B58" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="C58" s="10" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A59" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="A61" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="B61" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A62" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="B62" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="C62" s="19" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="57" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A57" s="11" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="10" t="s">
-        <v>166</v>
-      </c>
-      <c r="B58" s="19" t="s">
-        <v>131</v>
-      </c>
-      <c r="C58" s="10" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A61" s="11" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="19" t="s">
-        <v>131</v>
-      </c>
-      <c r="B62" s="10" t="s">
-        <v>139</v>
-      </c>
-      <c r="C62" s="19" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -1771,43 +1863,43 @@
       <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="20"/>
-      <c r="D1" s="21"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C1" s="21"/>
+      <c r="D1" s="22"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="23"/>
-    </row>
-    <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="23"/>
+      <c r="D2" s="24"/>
+    </row>
+    <row r="3" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="24"/>
-      <c r="D3" s="25"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C3" s="25"/>
+      <c r="D3" s="26"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>5</v>
       </c>
@@ -1821,7 +1913,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>10</v>
       </c>
@@ -1835,7 +1927,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>20</v>
       </c>
@@ -1846,10 +1938,10 @@
         <v>15</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>12</v>
       </c>
@@ -1860,10 +1952,10 @@
         <v>16</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>13</v>
       </c>
@@ -1874,13 +1966,13 @@
         <v>17</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G8" s="17" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G9" s="18" t="s">
         <v>0</v>
       </c>
@@ -1888,15 +1980,15 @@
         <v>72</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="20" t="s">
+      <c r="B10" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="20"/>
-      <c r="D10" s="21"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="22"/>
       <c r="G10" s="1" t="s">
         <v>71</v>
       </c>
@@ -1904,15 +1996,15 @@
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="22" t="s">
+      <c r="B11" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="22"/>
-      <c r="D11" s="23"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="24"/>
       <c r="G11" s="1" t="s">
         <v>1</v>
       </c>
@@ -1920,15 +2012,15 @@
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="24" t="s">
+      <c r="B12" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="C12" s="24"/>
-      <c r="D12" s="25"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="26"/>
       <c r="G12" s="1" t="s">
         <v>66</v>
       </c>
@@ -1936,7 +2028,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>5</v>
       </c>
@@ -1956,7 +2048,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>10</v>
       </c>
@@ -1976,7 +2068,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>20</v>
       </c>
@@ -1987,7 +2079,7 @@
         <v>43</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>69</v>
@@ -1996,7 +2088,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G16" s="1" t="s">
         <v>70</v>
       </c>
@@ -2004,37 +2096,37 @@
         <v>79</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B17" s="20" t="s">
+      <c r="B17" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="C17" s="20"/>
-      <c r="D17" s="21"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C17" s="21"/>
+      <c r="D17" s="22"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B18" s="22" t="s">
+      <c r="B18" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="C18" s="22"/>
-      <c r="D18" s="23"/>
-    </row>
-    <row r="19" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C18" s="23"/>
+      <c r="D18" s="24"/>
+    </row>
+    <row r="19" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B19" s="24" t="s">
+      <c r="B19" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="C19" s="24"/>
-      <c r="D19" s="25"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C19" s="25"/>
+      <c r="D19" s="26"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
         <v>5</v>
       </c>
@@ -2048,7 +2140,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>32</v>
       </c>
@@ -2062,7 +2154,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>25</v>
       </c>
@@ -2076,7 +2168,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>26</v>
       </c>
@@ -2087,10 +2179,10 @@
         <v>49</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="13" t="s">
         <v>27</v>
       </c>
@@ -2101,7 +2193,7 @@
         <v>50</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>82</v>
@@ -2110,7 +2202,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="13" t="s">
         <v>28</v>
       </c>
@@ -2121,7 +2213,7 @@
         <v>51</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>85</v>
@@ -2130,7 +2222,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="13" t="s">
         <v>35</v>
       </c>
@@ -2141,41 +2233,41 @@
         <v>52</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B28" s="20" t="s">
+      <c r="B28" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="C28" s="20"/>
-      <c r="D28" s="21"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C28" s="21"/>
+      <c r="D28" s="22"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B29" s="22" t="s">
+      <c r="B29" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="C29" s="22"/>
-      <c r="D29" s="23"/>
-    </row>
-    <row r="30" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C29" s="23"/>
+      <c r="D29" s="24"/>
+    </row>
+    <row r="30" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B30" s="24" t="s">
+      <c r="B30" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="C30" s="24"/>
-      <c r="D30" s="25"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C30" s="25"/>
+      <c r="D30" s="26"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="7" t="s">
         <v>5</v>
       </c>
@@ -2189,7 +2281,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="15" t="s">
         <v>23</v>
       </c>
@@ -2203,7 +2295,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>30</v>
       </c>
@@ -2217,7 +2309,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>31</v>
       </c>
@@ -2231,7 +2323,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>33</v>
       </c>
@@ -2242,10 +2334,10 @@
         <v>59</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="16" t="s">
         <v>35</v>
       </c>
@@ -2256,10 +2348,10 @@
         <v>60</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
         <v>38</v>
       </c>
@@ -2270,10 +2362,10 @@
         <v>61</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
         <v>39</v>
       </c>
@@ -2284,10 +2376,10 @@
         <v>62</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
         <v>80</v>
       </c>
@@ -2298,7 +2390,7 @@
         <v>81</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Correcion en las llaves foraneas
</commit_message>
<xml_diff>
--- a/Taller3_12_re.gonzalez10_ja.troconis10/docs/tablas.xlsx
+++ b/Taller3_12_re.gonzalez10_ja.troconis10/docs/tablas.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ricardo\Documents\SisTrans_VuelAndes_C12\Taller3_12_re.gonzalez10_ja.troconis10\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JavierAntonio\git\SisTrans_VuelAndes_C12\Taller3_12_re.gonzalez10_ja.troconis10\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="936" yWindow="0" windowWidth="23040" windowHeight="9396"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="23040" windowHeight="9390"/>
   </bookViews>
   <sheets>
     <sheet name="Esquema de Relación" sheetId="1" r:id="rId1"/>
@@ -460,12 +460,6 @@
     <t>carga</t>
   </si>
   <si>
-    <t>FK(Usuarios.tipoid)</t>
-  </si>
-  <si>
-    <t>FK(Usuarios.id)</t>
-  </si>
-  <si>
     <t>vuelo</t>
   </si>
   <si>
@@ -502,9 +496,6 @@
     <t>pais</t>
   </si>
   <si>
-    <t>FK(Paises.cod_pais)</t>
-  </si>
-  <si>
     <t>numero_de_serie</t>
   </si>
   <si>
@@ -563,12 +554,21 @@
   </si>
   <si>
     <t>ReservasPasajeros</t>
+  </si>
+  <si>
+    <t>PK2,FK(Usuarios.tipoid)</t>
+  </si>
+  <si>
+    <t>PK3,FK(Usuarios.id)</t>
+  </si>
+  <si>
+    <t>PK3,FK(Paises.cod_pais)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -881,7 +881,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -897,7 +897,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -972,6 +972,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1007,6 +1024,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1186,30 +1220,30 @@
   <dimension ref="A1:L63"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="B61" sqref="B61"/>
+      <selection activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.33203125" customWidth="1"/>
+    <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" customWidth="1"/>
     <col min="4" max="4" width="25" customWidth="1"/>
-    <col min="5" max="5" width="26.109375" customWidth="1"/>
-    <col min="6" max="6" width="29.44140625" customWidth="1"/>
-    <col min="7" max="7" width="27.33203125" customWidth="1"/>
+    <col min="5" max="5" width="26.140625" customWidth="1"/>
+    <col min="6" max="6" width="29.42578125" customWidth="1"/>
+    <col min="7" max="7" width="27.28515625" customWidth="1"/>
     <col min="8" max="8" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
         <v>24</v>
       </c>
       <c r="B1" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>25</v>
       </c>
@@ -1226,13 +1260,13 @@
         <v>35</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>47</v>
       </c>
@@ -1249,21 +1283,21 @@
         <v>88</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="18" x14ac:dyDescent="0.35">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
         <v>29</v>
       </c>
       <c r="B5" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>23</v>
       </c>
@@ -1274,16 +1308,16 @@
         <v>104</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="E6" s="10" t="s">
         <v>35</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="H6" s="10" t="s">
         <v>120</v>
@@ -1301,7 +1335,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
@@ -1312,22 +1346,22 @@
         <v>36</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>87</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>107</v>
@@ -1339,15 +1373,15 @@
         <v>110</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="18" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>10</v>
       </c>
@@ -1358,10 +1392,10 @@
         <v>111</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>21</v>
       </c>
@@ -1369,21 +1403,21 @@
         <v>22</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="18" x14ac:dyDescent="0.35">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
         <v>34</v>
       </c>
       <c r="B13" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>10</v>
       </c>
@@ -1394,7 +1428,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>21</v>
       </c>
@@ -1405,15 +1439,15 @@
         <v>118</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A17" s="11" t="s">
         <v>113</v>
       </c>
       <c r="B17" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="19" t="s">
         <v>117</v>
       </c>
@@ -1421,7 +1455,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>119</v>
       </c>
@@ -1429,15 +1463,15 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A21" s="11" t="s">
         <v>114</v>
       </c>
       <c r="B21" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="19" t="s">
         <v>116</v>
       </c>
@@ -1448,7 +1482,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>119</v>
       </c>
@@ -1459,24 +1493,24 @@
         <v>118</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A24" s="11"/>
     </row>
-    <row r="25" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A25" s="11" t="s">
         <v>112</v>
       </c>
       <c r="B25" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="E25" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
         <v>115</v>
       </c>
@@ -1490,7 +1524,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>21</v>
       </c>
@@ -1504,21 +1538,21 @@
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A29" s="11" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B29" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="D29" s="11" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="E29" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
         <v>115</v>
       </c>
@@ -1532,7 +1566,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>21</v>
       </c>
@@ -1546,12 +1580,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A33" s="11" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="10" t="s">
         <v>122</v>
       </c>
@@ -1565,10 +1599,10 @@
         <v>125</v>
       </c>
       <c r="E34" s="19" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>134</v>
       </c>
@@ -1585,21 +1619,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A37" s="11" t="s">
         <v>129</v>
       </c>
       <c r="B37" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="E37" s="11" t="s">
         <v>127</v>
       </c>
       <c r="F37" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="19" t="s">
         <v>122</v>
       </c>
@@ -1616,7 +1650,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>133</v>
       </c>
@@ -1633,21 +1667,21 @@
         <v>22</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A41" s="11" t="s">
         <v>138</v>
       </c>
       <c r="B41" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="E41" s="11" t="s">
         <v>135</v>
       </c>
       <c r="F41" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="19" t="s">
         <v>122</v>
       </c>
@@ -1661,7 +1695,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>133</v>
       </c>
@@ -1675,15 +1709,15 @@
         <v>22</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A45" s="11" t="s">
         <v>139</v>
       </c>
       <c r="B45" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="10" t="s">
         <v>123</v>
       </c>
@@ -1697,7 +1731,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>0</v>
       </c>
@@ -1711,15 +1745,15 @@
         <v>142</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A49" s="11" t="s">
         <v>144</v>
       </c>
       <c r="B49" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="19" t="s">
         <v>123</v>
       </c>
@@ -1733,35 +1767,35 @@
         <v>145</v>
       </c>
       <c r="E50" s="19" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E51" s="20" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A53" s="11" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B53" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="19" t="s">
         <v>123</v>
       </c>
@@ -1772,34 +1806,34 @@
         <v>130</v>
       </c>
       <c r="D54" s="19" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B55" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D55" s="20" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A57" s="11" t="s">
         <v>153</v>
       </c>
-      <c r="C55" s="1" t="s">
+      <c r="B57" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="10" t="s">
         <v>154</v>
-      </c>
-      <c r="D55" s="20" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A57" s="11" t="s">
-        <v>155</v>
-      </c>
-      <c r="B57" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A58" s="10" t="s">
-        <v>156</v>
       </c>
       <c r="B58" s="19" t="s">
         <v>122</v>
@@ -1808,26 +1842,26 @@
         <v>130</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>146</v>
+        <v>178</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A61" s="11" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B61" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="19" t="s">
         <v>122</v>
       </c>
@@ -1835,18 +1869,18 @@
         <v>130</v>
       </c>
       <c r="C62" s="19" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>146</v>
+        <v>133</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>147</v>
+        <v>132</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>160</v>
+        <v>180</v>
       </c>
     </row>
   </sheetData>
@@ -1863,13 +1897,13 @@
       <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -1879,7 +1913,7 @@
       <c r="C1" s="21"/>
       <c r="D1" s="22"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -1889,7 +1923,7 @@
       <c r="C2" s="23"/>
       <c r="D2" s="24"/>
     </row>
-    <row r="3" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -1899,7 +1933,7 @@
       <c r="C3" s="25"/>
       <c r="D3" s="26"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>5</v>
       </c>
@@ -1913,7 +1947,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>10</v>
       </c>
@@ -1927,7 +1961,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>20</v>
       </c>
@@ -1941,7 +1975,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>12</v>
       </c>
@@ -1955,7 +1989,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>13</v>
       </c>
@@ -1972,7 +2006,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G9" s="18" t="s">
         <v>0</v>
       </c>
@@ -1980,7 +2014,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>2</v>
       </c>
@@ -1996,7 +2030,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>3</v>
       </c>
@@ -2012,7 +2046,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>4</v>
       </c>
@@ -2028,7 +2062,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>5</v>
       </c>
@@ -2048,7 +2082,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>10</v>
       </c>
@@ -2068,7 +2102,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>20</v>
       </c>
@@ -2088,7 +2122,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G16" s="1" t="s">
         <v>70</v>
       </c>
@@ -2096,7 +2130,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>2</v>
       </c>
@@ -2106,7 +2140,7 @@
       <c r="C17" s="21"/>
       <c r="D17" s="22"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>3</v>
       </c>
@@ -2116,7 +2150,7 @@
       <c r="C18" s="23"/>
       <c r="D18" s="24"/>
     </row>
-    <row r="19" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>4</v>
       </c>
@@ -2126,7 +2160,7 @@
       <c r="C19" s="25"/>
       <c r="D19" s="26"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>5</v>
       </c>
@@ -2140,7 +2174,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>32</v>
       </c>
@@ -2154,7 +2188,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>25</v>
       </c>
@@ -2168,7 +2202,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>26</v>
       </c>
@@ -2182,7 +2216,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="13" t="s">
         <v>27</v>
       </c>
@@ -2202,7 +2236,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
         <v>28</v>
       </c>
@@ -2222,7 +2256,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
         <v>35</v>
       </c>
@@ -2236,8 +2270,8 @@
         <v>93</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>2</v>
       </c>
@@ -2247,7 +2281,7 @@
       <c r="C28" s="21"/>
       <c r="D28" s="22"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>3</v>
       </c>
@@ -2257,7 +2291,7 @@
       <c r="C29" s="23"/>
       <c r="D29" s="24"/>
     </row>
-    <row r="30" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
         <v>4</v>
       </c>
@@ -2267,7 +2301,7 @@
       <c r="C30" s="25"/>
       <c r="D30" s="26"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
         <v>5</v>
       </c>
@@ -2281,7 +2315,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="15" t="s">
         <v>23</v>
       </c>
@@ -2295,7 +2329,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>30</v>
       </c>
@@ -2309,7 +2343,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>31</v>
       </c>
@@ -2323,7 +2357,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>33</v>
       </c>
@@ -2337,7 +2371,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="16" t="s">
         <v>35</v>
       </c>
@@ -2351,7 +2385,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>38</v>
       </c>
@@ -2365,7 +2399,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
         <v>39</v>
       </c>
@@ -2379,7 +2413,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
         <v>80</v>
       </c>

</xml_diff>

<commit_message>
Actualizacion de las llaves y atributos. Solo falta la documentación.
Las tablas en el servidor ya han sido creadas
</commit_message>
<xml_diff>
--- a/Taller3_12_re.gonzalez10_ja.troconis10/docs/tablas.xlsx
+++ b/Taller3_12_re.gonzalez10_ja.troconis10/docs/tablas.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JavierAntonio\git\SisTrans_VuelAndes_C12\Taller3_12_re.gonzalez10_ja.troconis10\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ricardo\Documents\SisTrans_VuelAndes_C12\Taller3_12_re.gonzalez10_ja.troconis10\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="23040" windowHeight="9390"/>
+    <workbookView xWindow="936" yWindow="0" windowWidth="23040" windowHeight="9396"/>
   </bookViews>
   <sheets>
     <sheet name="Esquema de Relación" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="181">
   <si>
     <t>PK</t>
   </si>
@@ -328,9 +328,6 @@
     <t>NN,NC,CK(año_Fabricacion&gt;1970)</t>
   </si>
   <si>
-    <t>NULLABEL</t>
-  </si>
-  <si>
     <t>hora_Salida</t>
   </si>
   <si>
@@ -556,19 +553,22 @@
     <t>ReservasPasajeros</t>
   </si>
   <si>
+    <t>NULLABEL, CK(propiedad = Y|| propiedad = N|| propiedad isNULL)</t>
+  </si>
+  <si>
+    <t>PK3,FK(Paises.cod_pais)</t>
+  </si>
+  <si>
+    <t>PK3,FK(Usuarios.id)</t>
+  </si>
+  <si>
     <t>PK2,FK(Usuarios.tipoid)</t>
-  </si>
-  <si>
-    <t>PK3,FK(Usuarios.id)</t>
-  </si>
-  <si>
-    <t>PK3,FK(Paises.cod_pais)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -881,7 +881,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
+    <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -897,7 +897,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -972,23 +972,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1024,23 +1007,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1219,31 +1185,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="C63" sqref="C63"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="C67" sqref="C67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.28515625" customWidth="1"/>
+    <col min="1" max="1" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.33203125" customWidth="1"/>
     <col min="4" max="4" width="25" customWidth="1"/>
-    <col min="5" max="5" width="26.140625" customWidth="1"/>
-    <col min="6" max="6" width="29.42578125" customWidth="1"/>
-    <col min="7" max="7" width="27.28515625" customWidth="1"/>
+    <col min="5" max="5" width="26.109375" customWidth="1"/>
+    <col min="6" max="6" width="29.44140625" customWidth="1"/>
+    <col min="7" max="7" width="27.33203125" customWidth="1"/>
     <col min="8" max="8" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>24</v>
       </c>
       <c r="B1" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>25</v>
       </c>
@@ -1260,13 +1226,13 @@
         <v>35</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>47</v>
       </c>
@@ -1277,65 +1243,65 @@
         <v>101</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>102</v>
+        <v>177</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>88</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="18" x14ac:dyDescent="0.35">
       <c r="A5" s="11" t="s">
         <v>29</v>
       </c>
       <c r="B5" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>23</v>
       </c>
       <c r="B6" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="C6" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="C6" s="10" t="s">
-        <v>104</v>
-      </c>
       <c r="D6" s="10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E6" s="10" t="s">
         <v>35</v>
       </c>
       <c r="F6" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="G6" s="10" t="s">
         <v>160</v>
       </c>
-      <c r="G6" s="10" t="s">
-        <v>161</v>
-      </c>
       <c r="H6" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="I6" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="I6" s="10" t="s">
-        <v>121</v>
-      </c>
       <c r="J6" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="K6" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="K6" s="10" t="s">
-        <v>106</v>
-      </c>
       <c r="L6" s="10" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
@@ -1346,42 +1312,42 @@
         <v>36</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>87</v>
       </c>
       <c r="F7" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="G7" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="H7" s="1" t="s">
+      <c r="I7" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="I7" s="1" t="s">
-        <v>165</v>
-      </c>
       <c r="J7" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="K7" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="K7" s="1" t="s">
-        <v>108</v>
-      </c>
       <c r="L7" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="18" x14ac:dyDescent="0.35">
       <c r="A9" s="11" t="s">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
         <v>10</v>
       </c>
@@ -1389,13 +1355,13 @@
         <v>20</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>21</v>
       </c>
@@ -1403,21 +1369,21 @@
         <v>22</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:12" ht="18" x14ac:dyDescent="0.35">
       <c r="A13" s="11" t="s">
         <v>34</v>
       </c>
       <c r="B13" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
         <v>10</v>
       </c>
@@ -1425,10 +1391,10 @@
         <v>20</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>21</v>
       </c>
@@ -1436,95 +1402,95 @@
         <v>22</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A17" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B17" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="19" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B18" s="19" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A21" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B21" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="19" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B22" s="19" t="s">
         <v>20</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A24" s="11"/>
     </row>
-    <row r="25" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A25" s="11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B25" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E25" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B26" s="10" t="s">
         <v>20</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E26" s="10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>21</v>
       </c>
@@ -1538,35 +1504,35 @@
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A29" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="B29" t="s">
+        <v>165</v>
+      </c>
+      <c r="D29" s="11" t="s">
         <v>171</v>
       </c>
-      <c r="B29" t="s">
-        <v>166</v>
-      </c>
-      <c r="D29" s="11" t="s">
-        <v>172</v>
-      </c>
       <c r="E29" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B30" s="10" t="s">
         <v>20</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E30" s="10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>21</v>
       </c>
@@ -1580,82 +1546,85 @@
         <v>22</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A33" s="11" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+      <c r="B33" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="C34" s="19" t="s">
         <v>20</v>
       </c>
       <c r="D34" s="19" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E34" s="19" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A37" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="B37" t="s">
+        <v>165</v>
+      </c>
+      <c r="E37" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="F37" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="B38" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="B37" t="s">
-        <v>166</v>
-      </c>
-      <c r="E37" s="11" t="s">
+      <c r="C38" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="E38" s="10" t="s">
         <v>127</v>
-      </c>
-      <c r="F37" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="19" t="s">
-        <v>122</v>
-      </c>
-      <c r="B38" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="C38" s="10" t="s">
-        <v>137</v>
-      </c>
-      <c r="E38" s="10" t="s">
-        <v>128</v>
       </c>
       <c r="F38" s="10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>1</v>
@@ -1667,40 +1636,40 @@
         <v>22</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A41" s="11" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B41" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E41" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="F41" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="B42" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="E42" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="F42" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="F41" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="19" t="s">
-        <v>122</v>
-      </c>
-      <c r="B42" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="E42" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="F42" s="10" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>21</v>
@@ -1709,29 +1678,29 @@
         <v>22</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A45" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="B45" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="B46" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="B45" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="B46" s="10" t="s">
+      <c r="C46" s="19" t="s">
         <v>140</v>
       </c>
-      <c r="C46" s="19" t="s">
-        <v>141</v>
-      </c>
       <c r="D46" s="19" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>0</v>
       </c>
@@ -1739,148 +1708,148 @@
         <v>1</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A49" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="B49" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="B50" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="C50" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="D50" s="10" t="s">
         <v>144</v>
       </c>
-      <c r="B49" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="19" t="s">
-        <v>123</v>
-      </c>
-      <c r="B50" s="19" t="s">
-        <v>122</v>
-      </c>
-      <c r="C50" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="D50" s="10" t="s">
+      <c r="E50" s="19" t="s">
         <v>145</v>
       </c>
-      <c r="E50" s="19" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B51" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C51" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="C51" s="1" t="s">
-        <v>150</v>
-      </c>
       <c r="D51" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E51" s="20" t="s">
         <v>147</v>
       </c>
-      <c r="E51" s="20" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="53" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A53" s="11" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B53" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B54" s="19" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C54" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D54" s="19" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B55" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C55" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="C55" s="1" t="s">
+      <c r="D55" s="20" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="A57" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="D55" s="20" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A57" s="11" t="s">
+      <c r="B57" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A58" s="10" t="s">
         <v>153</v>
       </c>
-      <c r="B57" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="10" t="s">
+      <c r="B58" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="C58" s="10" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A59" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="B58" s="19" t="s">
-        <v>122</v>
-      </c>
-      <c r="C58" s="10" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
-        <v>155</v>
-      </c>
       <c r="B59" s="1" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A61" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="B61" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A62" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="B62" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="C62" s="19" t="s">
         <v>156</v>
       </c>
-      <c r="B61" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="19" t="s">
-        <v>122</v>
-      </c>
-      <c r="B62" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="C62" s="19" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -1897,13 +1866,13 @@
       <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -1913,7 +1882,7 @@
       <c r="C1" s="21"/>
       <c r="D1" s="22"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -1923,7 +1892,7 @@
       <c r="C2" s="23"/>
       <c r="D2" s="24"/>
     </row>
-    <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -1933,7 +1902,7 @@
       <c r="C3" s="25"/>
       <c r="D3" s="26"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>5</v>
       </c>
@@ -1947,7 +1916,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>10</v>
       </c>
@@ -1961,7 +1930,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>20</v>
       </c>
@@ -1975,7 +1944,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>12</v>
       </c>
@@ -1989,7 +1958,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>13</v>
       </c>
@@ -2006,7 +1975,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G9" s="18" t="s">
         <v>0</v>
       </c>
@@ -2014,7 +1983,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>2</v>
       </c>
@@ -2030,7 +1999,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>3</v>
       </c>
@@ -2046,7 +2015,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
         <v>4</v>
       </c>
@@ -2062,7 +2031,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>5</v>
       </c>
@@ -2082,7 +2051,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>10</v>
       </c>
@@ -2102,7 +2071,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>20</v>
       </c>
@@ -2122,7 +2091,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G16" s="1" t="s">
         <v>70</v>
       </c>
@@ -2130,7 +2099,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>2</v>
       </c>
@@ -2140,7 +2109,7 @@
       <c r="C17" s="21"/>
       <c r="D17" s="22"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>3</v>
       </c>
@@ -2150,7 +2119,7 @@
       <c r="C18" s="23"/>
       <c r="D18" s="24"/>
     </row>
-    <row r="19" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
         <v>4</v>
       </c>
@@ -2160,7 +2129,7 @@
       <c r="C19" s="25"/>
       <c r="D19" s="26"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
         <v>5</v>
       </c>
@@ -2174,7 +2143,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>32</v>
       </c>
@@ -2188,7 +2157,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>25</v>
       </c>
@@ -2202,7 +2171,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>26</v>
       </c>
@@ -2216,7 +2185,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="13" t="s">
         <v>27</v>
       </c>
@@ -2236,7 +2205,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="13" t="s">
         <v>28</v>
       </c>
@@ -2256,7 +2225,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="13" t="s">
         <v>35</v>
       </c>
@@ -2270,8 +2239,8 @@
         <v>93</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>2</v>
       </c>
@@ -2281,7 +2250,7 @@
       <c r="C28" s="21"/>
       <c r="D28" s="22"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>3</v>
       </c>
@@ -2291,7 +2260,7 @@
       <c r="C29" s="23"/>
       <c r="D29" s="24"/>
     </row>
-    <row r="30" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="4" t="s">
         <v>4</v>
       </c>
@@ -2301,7 +2270,7 @@
       <c r="C30" s="25"/>
       <c r="D30" s="26"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="7" t="s">
         <v>5</v>
       </c>
@@ -2315,7 +2284,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="15" t="s">
         <v>23</v>
       </c>
@@ -2329,7 +2298,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>30</v>
       </c>
@@ -2343,7 +2312,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>31</v>
       </c>
@@ -2357,7 +2326,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>33</v>
       </c>
@@ -2371,7 +2340,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="16" t="s">
         <v>35</v>
       </c>
@@ -2385,7 +2354,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
         <v>38</v>
       </c>
@@ -2399,7 +2368,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
         <v>39</v>
       </c>
@@ -2413,7 +2382,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
         <v>80</v>
       </c>

</xml_diff>